<commit_message>
updated the workload distribution
</commit_message>
<xml_diff>
--- a/final-project-workload.xlsx
+++ b/final-project-workload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD1BCC3-766C-40F3-B8D3-ADFA1869EB55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8898EF93-9B8F-4525-9C4B-BD887FF53995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -784,7 +784,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1221,13 +1221,13 @@
         <v>1.5</v>
       </c>
       <c r="D25" s="23">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="E25" s="11">
         <v>0</v>
       </c>
       <c r="F25" s="12">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G25" s="6">
         <f t="shared" si="1"/>
@@ -1307,7 +1307,7 @@
       </c>
       <c r="D29" s="20">
         <f>SUMPRODUCT($C19:$C28,D19:D28)/100</f>
-        <v>2.7450000000000001</v>
+        <v>1.9950000000000001</v>
       </c>
       <c r="E29" s="20">
         <f>SUMPRODUCT($C19:$C28,E19:E28)/100</f>
@@ -1315,7 +1315,7 @@
       </c>
       <c r="F29" s="20">
         <f>SUMPRODUCT($C19:$C28,F19:F28)/100</f>
-        <v>0</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -1325,7 +1325,7 @@
       <c r="C31" s="27"/>
       <c r="D31" s="28">
         <f>D$16+D29</f>
-        <v>8.74</v>
+        <v>7.99</v>
       </c>
       <c r="E31" s="28">
         <f>E$16+E29</f>
@@ -1333,7 +1333,7 @@
       </c>
       <c r="F31" s="29">
         <f>F$16+F29</f>
-        <v>6.0149999999999997</v>
+        <v>6.7649999999999997</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added student nrs to workload
</commit_message>
<xml_diff>
--- a/final-project-workload.xlsx
+++ b/final-project-workload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amand\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8898EF93-9B8F-4525-9C4B-BD887FF53995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901D1BFA-5FC1-4DBF-9F5E-26E34330C970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -784,7 +784,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -839,13 +839,13 @@
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="4">
-        <v>1</v>
+        <v>4829360</v>
       </c>
       <c r="E5" s="4">
-        <v>2</v>
+        <v>5079934</v>
       </c>
       <c r="F5" s="4">
-        <v>3</v>
+        <v>5336724</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>